<commit_message>
Implementing excel utility in framework
</commit_message>
<xml_diff>
--- a/Day_two/data.xlsx
+++ b/Day_two/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dines\Learn And Interview\Interview_question_answer\Day_two\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D29404E-988D-4C60-A57C-13E54BDF0B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE0F5EB-A1F9-4FD3-B72F-20800FE5B65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,37 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Roll no</t>
-  </si>
-  <si>
-    <t>Grade</t>
-  </si>
-  <si>
-    <t>Multipler</t>
-  </si>
-  <si>
-    <t>Dipak</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>ramesh</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>suresh</t>
-  </si>
-  <si>
-    <t>helesh</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Subject</t>
   </si>
@@ -66,6 +36,36 @@
   </si>
   <si>
     <t>Biology</t>
+  </si>
+  <si>
+    <t>GoingFrom</t>
+  </si>
+  <si>
+    <t>GoingTo</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Stops</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>JFK</t>
+  </si>
+  <si>
+    <t>1 Stop</t>
+  </si>
+  <si>
+    <t>2 Stop</t>
+  </si>
+  <si>
+    <t>0 Stop</t>
   </si>
 </sst>
 </file>
@@ -101,8 +101,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,78 +421,83 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45519</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45520</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45521</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="1">
+        <v>45522</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -515,15 +521,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>85</v>
@@ -531,7 +537,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -539,7 +545,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>45</v>

</xml_diff>